<commit_message>
Data updates to land/BLAPE and land/RPEpUACE
</commit_message>
<xml_diff>
--- a/InputData/land/RPEpUACE/Rebound Pol Emis per Unit Avoided CO2 Emis.xlsx
+++ b/InputData/land/RPEpUACE/Rebound Pol Emis per Unit Avoided CO2 Emis.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/land/rpepuace/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shelley\Dropbox (Energy Innovation)\PC (2)\Documents\GitHub_Repositories\eps-california\InputData\land\RPEpUACE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7F92AE-FC21-0D4A-936B-362E8F86FCEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2941C7E4-31FD-48AD-B888-7025CDC5C9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="19140" windowHeight="9260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13455" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="About" sheetId="4" r:id="rId1"/>
+    <sheet name="Data" sheetId="5" r:id="rId2"/>
     <sheet name="RPEpUACE" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>RPEpUACE Rebound Pollutant Emissions per Unit Avoided CO2 Emissions</t>
   </si>
@@ -41,12 +41,6 @@
     <t>Source:</t>
   </si>
   <si>
-    <t>http://www.epa.gov/climatechange/Downloads/ghgemissions/US-GHG-Inventory-2015-Main-Text.pdf</t>
-  </si>
-  <si>
-    <t>Page 6-4, Table 6-3</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -116,10 +110,19 @@
     <t>F gases</t>
   </si>
   <si>
-    <t>Inventory of U.S. Greenhouse Gas Emissions and Sinks: 1990-2013</t>
-  </si>
-  <si>
     <t>Rebound Emis Factor (dimensionless)</t>
+  </si>
+  <si>
+    <t>Draft Inventory of US Greenhouse Gas Emissions Emissions and Sinks</t>
+  </si>
+  <si>
+    <t>https://www.epa.gov/sites/production/files/2021-02/documents/us-ghg-inventory-2021-main-text.pdf</t>
+  </si>
+  <si>
+    <t>Page 470, Table 6-3</t>
+  </si>
+  <si>
+    <t>data/file updated:</t>
   </si>
 </sst>
 </file>
@@ -519,239 +522,250 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D87D418-2159-4E13-81ED-7D41107B32BC}">
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5">
-        <v>44307</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="5">
+        <v>44481</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B4" s="4">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{CDA1410F-ADEC-4605-951E-E83E63C5B9CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A64F3CF-34D6-4281-835E-34695CCFD3F5}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" customWidth="1"/>
+    <col min="12" max="12" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>2015</v>
+      </c>
+      <c r="C3">
+        <v>2016</v>
+      </c>
+      <c r="D3">
+        <v>2017</v>
+      </c>
+      <c r="E3">
+        <v>2018</v>
+      </c>
+      <c r="F3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>-791695</v>
+      </c>
+      <c r="C4">
+        <v>-855998</v>
+      </c>
+      <c r="D4">
+        <v>-792046</v>
+      </c>
+      <c r="E4">
+        <v>-824885</v>
+      </c>
+      <c r="F4">
+        <v>-812695</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B5">
+        <v>663</v>
+      </c>
+      <c r="C5">
+        <v>308</v>
+      </c>
+      <c r="D5">
+        <v>614</v>
+      </c>
+      <c r="E5">
+        <v>552</v>
+      </c>
+      <c r="F5">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>38</v>
+      </c>
+      <c r="C6">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>36</v>
+      </c>
+      <c r="E6">
+        <v>32</v>
+      </c>
+      <c r="F6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <f>B5/B4</f>
+        <v>-8.3744371254081433E-4</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:F8" si="0">C5/C4</f>
+        <v>-3.5981392479888971E-4</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-7.7520750057446164E-4</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>-6.6918418931123734E-4</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>-6.7922160220008736E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3">
-        <v>2009</v>
-      </c>
-      <c r="C3">
-        <v>2010</v>
-      </c>
-      <c r="D3">
-        <v>2011</v>
-      </c>
-      <c r="E3">
-        <v>2012</v>
-      </c>
-      <c r="F3">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>-862631</v>
-      </c>
-      <c r="C4">
-        <v>-862025</v>
-      </c>
-      <c r="D4">
-        <v>-872103</v>
-      </c>
-      <c r="E4">
-        <v>-869580</v>
-      </c>
-      <c r="F4">
-        <v>-871026</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>234</v>
-      </c>
-      <c r="C5">
-        <v>190</v>
-      </c>
-      <c r="D5">
-        <v>584</v>
-      </c>
-      <c r="E5">
-        <v>627</v>
-      </c>
-      <c r="F5">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>22</v>
-      </c>
-      <c r="C6">
-        <v>20</v>
-      </c>
-      <c r="D6">
-        <v>42</v>
-      </c>
-      <c r="E6">
-        <v>45</v>
-      </c>
-      <c r="F6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="3">
-        <f>B5/B4</f>
-        <v>-2.7126314727850032E-4</v>
-      </c>
-      <c r="C8" s="3">
-        <f t="shared" ref="C8:F8" si="0">C5/C4</f>
-        <v>-2.2041124097328964E-4</v>
-      </c>
-      <c r="D8" s="3">
-        <f t="shared" si="0"/>
-        <v>-6.6964567258683894E-4</v>
-      </c>
-      <c r="E8" s="3">
-        <f t="shared" si="0"/>
-        <v>-7.2103774235837996E-4</v>
-      </c>
-      <c r="F8" s="3">
-        <f t="shared" si="0"/>
-        <v>-2.6750062569888842E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <f>B6/B4</f>
-        <v>-2.5503372821055586E-5</v>
-      </c>
-      <c r="C9" s="3">
-        <f t="shared" ref="C9:F9" si="1">C6/C4</f>
-        <v>-2.3201183260346277E-5</v>
-      </c>
-      <c r="D9" s="3">
+        <v>-4.7998282166743506E-5</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:G9" si="1">C6/C4</f>
+        <v>-2.1028086514220829E-5</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="1"/>
-        <v>-4.8159449055902798E-5</v>
-      </c>
-      <c r="E9" s="3">
+        <v>-4.5451905571141073E-5</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="1"/>
-        <v>-5.1749120264955494E-5</v>
-      </c>
-      <c r="F9" s="3">
+        <v>-3.8793286336883321E-5</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="1"/>
-        <v>-2.6405641163409588E-5</v>
+        <v>-3.9375165344932599E-5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -763,112 +777,112 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
       <c r="B10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3">
         <f>-AVERAGE(Data!B8:F8)</f>
-        <v>4.2997168577917945E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>6.6417418588509813E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3">
         <f>-AVERAGE(Data!B9:F9)</f>
-        <v>3.5003753313133949E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3.8529345186784264E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>0</v>

</xml_diff>